<commit_message>
Terminated the validation phase (everything is on the Results/Validation folder and can be checked there); re-runned the GeneticHeuristic algorithm with the files in which we had the model result (in /Results/Comparisons)
</commit_message>
<xml_diff>
--- a/PolynomialKnapsackProblem/Updated_folder/Results/Comparisons/Second_configs_comparison.xlsx
+++ b/PolynomialKnapsackProblem/Updated_folder/Results/Comparisons/Second_configs_comparison.xlsx
@@ -1,26 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23524"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alebaldus/Desktop/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3319823E-3F11-3E40-923B-B13547C899FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{11997680-2F3E-4D52-9212-F7BB2E64FE4C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="25360" windowHeight="15280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191028" calcCompleted="0"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="54">
   <si>
     <t>Name</t>
   </si>
@@ -28,31 +34,40 @@
     <t>Result_Model</t>
   </si>
   <si>
-    <t>Result_Heu</t>
-  </si>
-  <si>
-    <t>Result_Heu2</t>
-  </si>
-  <si>
-    <t>PercentageResHeu1</t>
-  </si>
-  <si>
-    <t>PercentageResHeu2</t>
+    <t>Result_HeuNM</t>
+  </si>
+  <si>
+    <t>Result_HeuM</t>
+  </si>
+  <si>
+    <t>PercentageResHeuNM</t>
+  </si>
+  <si>
+    <t>PercentageResHeuM</t>
   </si>
   <si>
     <t>Time_Model</t>
   </si>
   <si>
-    <t>Time_Heu</t>
-  </si>
-  <si>
-    <t>Time_Heu2</t>
-  </si>
-  <si>
-    <t>Diff_Time_Model_Heu</t>
-  </si>
-  <si>
-    <t>Diff_Time_Model_Heu2</t>
+    <t>Time_HeuNM</t>
+  </si>
+  <si>
+    <t>Time_HeuM</t>
+  </si>
+  <si>
+    <t>Diff_Time_Model_Heu_NM</t>
+  </si>
+  <si>
+    <t>Diff_Time_Model_Heu_M</t>
+  </si>
+  <si>
+    <t>M&gt;NM(RES)</t>
+  </si>
+  <si>
+    <t>Count</t>
+  </si>
+  <si>
+    <t>M&lt;NM(TIME)</t>
   </si>
   <si>
     <t>S_700_329_5867.825.json</t>
@@ -179,7 +194,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -231,20 +246,39 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -279,7 +313,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -599,43 +633,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L41"/>
+  <dimension ref="A1:Q41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:L1048576"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="24" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="17" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="H1" s="1" t="s">
@@ -653,28 +689,40 @@
       <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="N1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="3">
+        <v>14</v>
+      </c>
+      <c r="C2">
         <v>20559</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2">
         <v>20149.224296151591</v>
       </c>
-      <c r="E2" s="3">
-        <v>20135.611587997992</v>
-      </c>
-      <c r="F2" s="3">
+      <c r="E2">
+        <v>20091.6770746248</v>
+      </c>
+      <c r="F2">
         <v>1.9931694335736602E-2</v>
       </c>
-      <c r="G2" s="3">
-        <v>2.0593823240527848E-2</v>
+      <c r="G2">
+        <v>2.2730819853845199E-2</v>
       </c>
       <c r="H2">
         <v>722</v>
@@ -683,36 +731,52 @@
         <v>12.446</v>
       </c>
       <c r="J2">
-        <v>7.1520000000000001</v>
+        <v>11.391999999999999</v>
       </c>
       <c r="K2">
         <v>709.55399999999997</v>
       </c>
       <c r="L2">
-        <v>714.84799999999996</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+        <v>710.60799999999995</v>
+      </c>
+      <c r="N2">
+        <f>IF(G2&lt;=F2,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <f>SUM(N2:N41)</f>
+        <v>15</v>
+      </c>
+      <c r="P2" s="4">
+        <f>IF(J2&lt;I2,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="Q2" s="2">
+        <f>SUM(P2:P41)</f>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="3">
+        <v>15</v>
+      </c>
+      <c r="C3">
         <v>28577</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3">
         <v>27709.00024677697</v>
       </c>
-      <c r="E3" s="3">
-        <v>27618.9591985609</v>
-      </c>
-      <c r="F3" s="3">
+      <c r="E3">
+        <v>27528.180400980309</v>
+      </c>
+      <c r="F3">
         <v>3.037406841946438E-2</v>
       </c>
-      <c r="G3" s="3">
-        <v>3.3524890696682762E-2</v>
+      <c r="G3">
+        <v>3.6701529167501523E-2</v>
       </c>
       <c r="H3">
         <v>742</v>
@@ -721,36 +785,44 @@
         <v>5.9720000000000004</v>
       </c>
       <c r="J3">
-        <v>3.673</v>
+        <v>4.2380000000000004</v>
       </c>
       <c r="K3">
         <v>736.02800000000002</v>
       </c>
       <c r="L3">
-        <v>738.327</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+        <v>737.76199999999994</v>
+      </c>
+      <c r="N3">
+        <f t="shared" ref="N3:N41" si="0">IF(G3&lt;=F3,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <f t="shared" ref="P3:P41" si="1">IF(J3&lt;I3,1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="3">
+        <v>16</v>
+      </c>
+      <c r="C4">
         <v>12112</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4">
         <v>11672.20203362658</v>
       </c>
-      <c r="E4" s="3">
-        <v>11686.172726113889</v>
-      </c>
-      <c r="F4" s="3">
+      <c r="E4">
+        <v>11712.852310595659</v>
+      </c>
+      <c r="F4">
         <v>3.6310928531490823E-2</v>
       </c>
-      <c r="G4" s="3">
-        <v>3.5157469772631622E-2</v>
+      <c r="G4">
+        <v>3.295472997063565E-2</v>
       </c>
       <c r="H4">
         <v>632</v>
@@ -759,36 +831,44 @@
         <v>6.4820000000000002</v>
       </c>
       <c r="J4">
-        <v>3.9260000000000002</v>
+        <v>4.3460000000000001</v>
       </c>
       <c r="K4">
         <v>625.51800000000003</v>
       </c>
       <c r="L4">
-        <v>628.07399999999996</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+        <v>627.654</v>
+      </c>
+      <c r="N4">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="P4">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="3">
+        <v>17</v>
+      </c>
+      <c r="C5">
         <v>2751</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5">
         <v>2602.792710062859</v>
       </c>
-      <c r="E5" s="3">
-        <v>2622.141037058836</v>
-      </c>
-      <c r="F5" s="3">
+      <c r="E5">
+        <v>2654.2435932398339</v>
+      </c>
+      <c r="F5">
         <v>5.3873969442799353E-2</v>
       </c>
-      <c r="G5" s="3">
-        <v>4.684077169798781E-2</v>
+      <c r="G5">
+        <v>3.5171358327941153E-2</v>
       </c>
       <c r="H5">
         <v>919</v>
@@ -797,36 +877,44 @@
         <v>3.4000000000000002E-2</v>
       </c>
       <c r="J5">
-        <v>0.109</v>
+        <v>0.13900000000000001</v>
       </c>
       <c r="K5">
         <v>918.96600000000001</v>
       </c>
       <c r="L5">
-        <v>918.89099999999996</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+        <v>918.86099999999999</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="3">
+        <v>18</v>
+      </c>
+      <c r="C6">
         <v>26381</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6">
         <v>25366.495838850529</v>
       </c>
-      <c r="E6" s="3">
-        <v>25328.0871620258</v>
-      </c>
-      <c r="F6" s="3">
+      <c r="E6">
+        <v>25256.71388630971</v>
+      </c>
+      <c r="F6">
         <v>3.8455864491469878E-2</v>
       </c>
-      <c r="G6" s="3">
-        <v>3.9911786436230473E-2</v>
+      <c r="G6">
+        <v>4.2617266733266143E-2</v>
       </c>
       <c r="H6">
         <v>383</v>
@@ -835,36 +923,44 @@
         <v>5.4509999999999996</v>
       </c>
       <c r="J6">
-        <v>3.03</v>
+        <v>3.2970000000000002</v>
       </c>
       <c r="K6">
         <v>377.54899999999998</v>
       </c>
       <c r="L6">
-        <v>379.97</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+        <v>379.70299999999997</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="3">
+        <v>19</v>
+      </c>
+      <c r="C7">
         <v>37440</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7">
         <v>36354.415159351323</v>
       </c>
-      <c r="E7" s="3">
-        <v>36333.999846920953</v>
-      </c>
-      <c r="F7" s="3">
+      <c r="E7">
+        <v>36109.267991973851</v>
+      </c>
+      <c r="F7">
         <v>2.8995321598522351E-2</v>
       </c>
-      <c r="G7" s="3">
-        <v>2.9540602379248049E-2</v>
+      <c r="G7">
+        <v>3.5543055769929187E-2</v>
       </c>
       <c r="H7">
         <v>992</v>
@@ -873,36 +969,44 @@
         <v>7.7240000000000002</v>
       </c>
       <c r="J7">
-        <v>5.0599999999999996</v>
+        <v>6.0090000000000003</v>
       </c>
       <c r="K7">
         <v>984.27599999999995</v>
       </c>
       <c r="L7">
-        <v>986.94</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+        <v>985.99099999999999</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="3">
+        <v>20</v>
+      </c>
+      <c r="C8">
         <v>2795</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8">
         <v>2706.912720906475</v>
       </c>
-      <c r="E8" s="3">
-        <v>2706.912720906475</v>
-      </c>
-      <c r="F8" s="3">
+      <c r="E8">
+        <v>2730.0640799129869</v>
+      </c>
+      <c r="F8">
         <v>3.1516021142584977E-2</v>
       </c>
-      <c r="G8" s="3">
-        <v>3.1516021142584977E-2</v>
+      <c r="G8">
+        <v>2.3232887329879291E-2</v>
       </c>
       <c r="H8">
         <v>586</v>
@@ -911,36 +1015,44 @@
         <v>0.154</v>
       </c>
       <c r="J8">
-        <v>0.14099999999999999</v>
+        <v>0.18</v>
       </c>
       <c r="K8">
         <v>585.846</v>
       </c>
       <c r="L8">
-        <v>585.85900000000004</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+        <v>585.82000000000005</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="3">
+        <v>21</v>
+      </c>
+      <c r="C9">
         <v>36819</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9">
         <v>35696.008172707763</v>
       </c>
-      <c r="E9" s="3">
-        <v>35706.764753306386</v>
-      </c>
-      <c r="F9" s="3">
+      <c r="E9">
+        <v>35650.573245114269</v>
+      </c>
+      <c r="F9">
         <v>3.050033480790473E-2</v>
       </c>
-      <c r="G9" s="3">
-        <v>3.0208187259121819E-2</v>
+      <c r="G9">
+        <v>3.1734342455952948E-2</v>
       </c>
       <c r="H9">
         <v>512</v>
@@ -949,36 +1061,44 @@
         <v>9.5239999999999991</v>
       </c>
       <c r="J9">
-        <v>6.1310000000000002</v>
+        <v>8.2129999999999992</v>
       </c>
       <c r="K9">
         <v>502.476</v>
       </c>
       <c r="L9">
-        <v>505.86900000000003</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+        <v>503.78699999999998</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="3">
+        <v>22</v>
+      </c>
+      <c r="C10">
         <v>26168</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10">
         <v>25504.074031227821</v>
       </c>
-      <c r="E10" s="3">
-        <v>25515.2156479396</v>
-      </c>
-      <c r="F10" s="3">
+      <c r="E10">
+        <v>25519.602976987349</v>
+      </c>
+      <c r="F10">
         <v>2.5371674135286699E-2</v>
       </c>
-      <c r="G10" s="3">
-        <v>2.494590156146425E-2</v>
+      <c r="G10">
+        <v>2.4778241478624681E-2</v>
       </c>
       <c r="H10">
         <v>72</v>
@@ -987,36 +1107,44 @@
         <v>0.26300000000000001</v>
       </c>
       <c r="J10">
-        <v>4.6159999999999997</v>
+        <v>7.6689999999999996</v>
       </c>
       <c r="K10">
         <v>71.736999999999995</v>
       </c>
       <c r="L10">
-        <v>67.384</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+        <v>64.331000000000003</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="P10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="3">
+        <v>23</v>
+      </c>
+      <c r="C11">
         <v>31420</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11">
         <v>30621.538956153268</v>
       </c>
-      <c r="E11" s="3">
-        <v>30677.651388351191</v>
-      </c>
-      <c r="F11" s="3">
+      <c r="E11">
+        <v>30567.886606146811</v>
+      </c>
+      <c r="F11">
         <v>2.5412509352219219E-2</v>
       </c>
-      <c r="G11" s="3">
-        <v>2.3626626723386789E-2</v>
+      <c r="G11">
+        <v>2.712009528495192E-2</v>
       </c>
       <c r="H11">
         <v>409</v>
@@ -1025,36 +1153,44 @@
         <v>10.098000000000001</v>
       </c>
       <c r="J11">
-        <v>5.7469999999999999</v>
+        <v>8.3559999999999999</v>
       </c>
       <c r="K11">
         <v>398.90199999999999</v>
       </c>
       <c r="L11">
-        <v>403.25299999999999</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+        <v>400.64400000000001</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17">
       <c r="A12" s="1">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="3">
+        <v>24</v>
+      </c>
+      <c r="C12">
         <v>3041</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12">
         <v>2941.7736935174912</v>
       </c>
-      <c r="E12" s="3">
-        <v>2941.7736935174912</v>
-      </c>
-      <c r="F12" s="3">
+      <c r="E12">
+        <v>2989.199946362935</v>
+      </c>
+      <c r="F12">
         <v>3.2629499007730607E-2</v>
       </c>
-      <c r="G12" s="3">
-        <v>3.2629499007730607E-2</v>
+      <c r="G12">
+        <v>1.7033888075325569E-2</v>
       </c>
       <c r="H12">
         <v>17</v>
@@ -1063,36 +1199,44 @@
         <v>3.4000000000000002E-2</v>
       </c>
       <c r="J12">
-        <v>0.10199999999999999</v>
+        <v>0.13100000000000001</v>
       </c>
       <c r="K12">
         <v>16.966000000000001</v>
       </c>
       <c r="L12">
-        <v>16.898</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+        <v>16.869</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="P12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17">
       <c r="A13" s="1">
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" s="3">
+        <v>25</v>
+      </c>
+      <c r="C13">
         <v>2423</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13">
         <v>2249.188179492975</v>
       </c>
-      <c r="E13" s="3">
-        <v>2323.2647437588221</v>
-      </c>
-      <c r="F13" s="3">
+      <c r="E13">
+        <v>2310.0910551429538</v>
+      </c>
+      <c r="F13">
         <v>7.1734139705747199E-2</v>
       </c>
-      <c r="G13" s="3">
-        <v>4.1161888667427947E-2</v>
+      <c r="G13">
+        <v>4.6598821649626997E-2</v>
       </c>
       <c r="H13">
         <v>56</v>
@@ -1101,36 +1245,44 @@
         <v>0.13300000000000001</v>
       </c>
       <c r="J13">
-        <v>0.13900000000000001</v>
+        <v>0.23</v>
       </c>
       <c r="K13">
         <v>55.866999999999997</v>
       </c>
       <c r="L13">
-        <v>55.860999999999997</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+        <v>55.77</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="P13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17">
       <c r="A14" s="1">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14" s="3">
+        <v>26</v>
+      </c>
+      <c r="C14">
         <v>37778</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14">
         <v>36972.637391015684</v>
       </c>
-      <c r="E14" s="3">
-        <v>37063.683740941087</v>
-      </c>
-      <c r="F14" s="3">
+      <c r="E14">
+        <v>36825.976694882163</v>
+      </c>
+      <c r="F14">
         <v>2.1318296600781501E-2</v>
       </c>
-      <c r="G14" s="3">
-        <v>1.8908260338263351E-2</v>
+      <c r="G14">
+        <v>2.520046866212727E-2</v>
       </c>
       <c r="H14">
         <v>313</v>
@@ -1139,36 +1291,44 @@
         <v>10.766999999999999</v>
       </c>
       <c r="J14">
-        <v>6.3330000000000002</v>
+        <v>9.5570000000000004</v>
       </c>
       <c r="K14">
         <v>302.233</v>
       </c>
       <c r="L14">
-        <v>306.66699999999997</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+        <v>303.44299999999998</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P14">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17">
       <c r="A15" s="1">
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15" s="3">
+        <v>27</v>
+      </c>
+      <c r="C15">
         <v>8571</v>
       </c>
-      <c r="D15" s="3">
+      <c r="D15">
         <v>8262.3590848892691</v>
       </c>
-      <c r="E15" s="3">
-        <v>8214.6715213095449</v>
-      </c>
-      <c r="F15" s="3">
+      <c r="E15">
+        <v>8261.3245337568715</v>
+      </c>
+      <c r="F15">
         <v>3.6009907258281522E-2</v>
       </c>
-      <c r="G15" s="3">
-        <v>4.1573734533946458E-2</v>
+      <c r="G15">
+        <v>3.6130610925577941E-2</v>
       </c>
       <c r="H15">
         <v>491</v>
@@ -1177,36 +1337,44 @@
         <v>3.3090000000000002</v>
       </c>
       <c r="J15">
-        <v>1.8380000000000001</v>
+        <v>2.2639999999999998</v>
       </c>
       <c r="K15">
         <v>487.69099999999997</v>
       </c>
       <c r="L15">
-        <v>489.16199999999998</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+        <v>488.73599999999999</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P15">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17">
       <c r="A16" s="1">
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>25</v>
-      </c>
-      <c r="C16" s="3">
+        <v>28</v>
+      </c>
+      <c r="C16">
         <v>14112</v>
       </c>
-      <c r="D16" s="3">
+      <c r="D16">
         <v>13794.774955458681</v>
       </c>
-      <c r="E16" s="3">
-        <v>13813.140849903</v>
-      </c>
-      <c r="F16" s="3">
+      <c r="E16">
+        <v>13843.717919241721</v>
+      </c>
+      <c r="F16">
         <v>2.2479098961261029E-2</v>
       </c>
-      <c r="G16" s="3">
-        <v>2.1177660862882371E-2</v>
+      <c r="G16">
+        <v>1.9010918421080141E-2</v>
       </c>
       <c r="H16">
         <v>286</v>
@@ -1215,36 +1383,44 @@
         <v>0.74199999999999999</v>
       </c>
       <c r="J16">
-        <v>1.381</v>
+        <v>3.6419999999999999</v>
       </c>
       <c r="K16">
         <v>285.25799999999998</v>
       </c>
       <c r="L16">
-        <v>284.61900000000003</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+        <v>282.358</v>
+      </c>
+      <c r="N16">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="P16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16">
       <c r="A17" s="1">
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>26</v>
-      </c>
-      <c r="C17" s="3">
+        <v>29</v>
+      </c>
+      <c r="C17">
         <v>31574</v>
       </c>
-      <c r="D17" s="3">
+      <c r="D17">
         <v>30448.242898714259</v>
       </c>
-      <c r="E17" s="3">
-        <v>30250.009860876849</v>
-      </c>
-      <c r="F17" s="3">
+      <c r="E17">
+        <v>30280.66659631567</v>
+      </c>
+      <c r="F17">
         <v>3.565456075523344E-2</v>
       </c>
-      <c r="G17" s="3">
-        <v>4.193292389697708E-2</v>
+      <c r="G17">
+        <v>4.0961975159445427E-2</v>
       </c>
       <c r="H17">
         <v>803</v>
@@ -1253,36 +1429,44 @@
         <v>5.16</v>
       </c>
       <c r="J17">
-        <v>3.8889999999999998</v>
+        <v>3.9529999999999998</v>
       </c>
       <c r="K17">
         <v>797.84</v>
       </c>
       <c r="L17">
-        <v>799.11099999999999</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+        <v>799.04700000000003</v>
+      </c>
+      <c r="N17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P17">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16">
       <c r="A18" s="1">
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>27</v>
-      </c>
-      <c r="C18" s="3">
+        <v>30</v>
+      </c>
+      <c r="C18">
         <v>17245</v>
       </c>
-      <c r="D18" s="3">
+      <c r="D18">
         <v>16852.01299448956</v>
       </c>
-      <c r="E18" s="3">
-        <v>16701.841510465871</v>
-      </c>
-      <c r="F18" s="3">
+      <c r="E18">
+        <v>16764.24529691138</v>
+      </c>
+      <c r="F18">
         <v>2.278846074284974E-2</v>
       </c>
-      <c r="G18" s="3">
-        <v>3.1496578111575857E-2</v>
+      <c r="G18">
+        <v>2.787791841627232E-2</v>
       </c>
       <c r="H18">
         <v>33</v>
@@ -1291,36 +1475,44 @@
         <v>7.3170000000000002</v>
       </c>
       <c r="J18">
-        <v>4.234</v>
+        <v>5.3339999999999996</v>
       </c>
       <c r="K18">
         <v>25.683</v>
       </c>
       <c r="L18">
-        <v>28.765999999999998</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+        <v>27.666</v>
+      </c>
+      <c r="N18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P18">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16">
       <c r="A19" s="1">
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>28</v>
-      </c>
-      <c r="C19" s="3">
+        <v>31</v>
+      </c>
+      <c r="C19">
         <v>26190</v>
       </c>
-      <c r="D19" s="3">
+      <c r="D19">
         <v>25550.771795266079</v>
       </c>
-      <c r="E19" s="3">
-        <v>25592.66015481373</v>
-      </c>
-      <c r="F19" s="3">
+      <c r="E19">
+        <v>25531.131339859061</v>
+      </c>
+      <c r="F19">
         <v>2.440733885963808E-2</v>
       </c>
-      <c r="G19" s="3">
-        <v>2.280793605140399E-2</v>
+      <c r="G19">
+        <v>2.5157260791941301E-2</v>
       </c>
       <c r="H19">
         <v>826</v>
@@ -1329,36 +1521,44 @@
         <v>7.2709999999999999</v>
       </c>
       <c r="J19">
-        <v>4.3680000000000003</v>
+        <v>5.9290000000000003</v>
       </c>
       <c r="K19">
         <v>818.72900000000004</v>
       </c>
       <c r="L19">
-        <v>821.63199999999995</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+        <v>820.07100000000003</v>
+      </c>
+      <c r="N19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P19">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16">
       <c r="A20" s="1">
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>29</v>
-      </c>
-      <c r="C20" s="3">
+        <v>32</v>
+      </c>
+      <c r="C20">
         <v>3324</v>
       </c>
-      <c r="D20" s="3">
+      <c r="D20">
         <v>3271.751903125476</v>
       </c>
-      <c r="E20" s="3">
-        <v>3236.456294948292</v>
-      </c>
-      <c r="F20" s="3">
+      <c r="E20">
+        <v>3278.0581059219198</v>
+      </c>
+      <c r="F20">
         <v>1.5718440696306991E-2</v>
       </c>
-      <c r="G20" s="3">
-        <v>2.6336854708696619E-2</v>
+      <c r="G20">
+        <v>1.382126777318898E-2</v>
       </c>
       <c r="H20">
         <v>924</v>
@@ -1367,36 +1567,44 @@
         <v>0.45300000000000001</v>
       </c>
       <c r="J20">
-        <v>0.29599999999999999</v>
+        <v>0.4</v>
       </c>
       <c r="K20">
         <v>923.54700000000003</v>
       </c>
       <c r="L20">
-        <v>923.70399999999995</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+        <v>923.6</v>
+      </c>
+      <c r="N20">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="P20">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16">
       <c r="A21" s="1">
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>30</v>
-      </c>
-      <c r="C21" s="3">
+        <v>33</v>
+      </c>
+      <c r="C21">
         <v>2623</v>
       </c>
-      <c r="D21" s="3">
+      <c r="D21">
         <v>2464.0324885606428</v>
       </c>
-      <c r="E21" s="3">
-        <v>2500.4518124042279</v>
-      </c>
-      <c r="F21" s="3">
+      <c r="E21">
+        <v>2510.3939442623468</v>
+      </c>
+      <c r="F21">
         <v>6.0605227388241388E-2</v>
       </c>
-      <c r="G21" s="3">
-        <v>4.6720620509253387E-2</v>
+      <c r="G21">
+        <v>4.2930253807721371E-2</v>
       </c>
       <c r="H21">
         <v>491</v>
@@ -1413,28 +1621,36 @@
       <c r="L21">
         <v>490.87799999999999</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="N21">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="P21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16">
       <c r="A22" s="1">
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>31</v>
-      </c>
-      <c r="C22" s="3">
+        <v>34</v>
+      </c>
+      <c r="C22">
         <v>22732</v>
       </c>
-      <c r="D22" s="3">
+      <c r="D22">
         <v>22313.191820123451</v>
       </c>
-      <c r="E22" s="3">
-        <v>22241.260003673931</v>
-      </c>
-      <c r="F22" s="3">
+      <c r="E22">
+        <v>22233.30881296171</v>
+      </c>
+      <c r="F22">
         <v>1.8423727779190241E-2</v>
       </c>
-      <c r="G22" s="3">
-        <v>2.1588069519886881E-2</v>
+      <c r="G22">
+        <v>2.19378491570601E-2</v>
       </c>
       <c r="H22">
         <v>925</v>
@@ -1443,36 +1659,44 @@
         <v>10.351000000000001</v>
       </c>
       <c r="J22">
-        <v>6.3609999999999998</v>
+        <v>8.5449999999999999</v>
       </c>
       <c r="K22">
         <v>914.649</v>
       </c>
       <c r="L22">
-        <v>918.63900000000001</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+        <v>916.45500000000004</v>
+      </c>
+      <c r="N22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P22">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16">
       <c r="A23" s="1">
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>32</v>
-      </c>
-      <c r="C23" s="3">
+        <v>35</v>
+      </c>
+      <c r="C23">
         <v>49809</v>
       </c>
-      <c r="D23" s="3">
+      <c r="D23">
         <v>-1</v>
       </c>
-      <c r="E23" s="3">
-        <v>-1</v>
-      </c>
-      <c r="F23" s="3">
+      <c r="E23">
+        <v>46697.180889345182</v>
+      </c>
+      <c r="F23">
         <v>1.000020076692967</v>
       </c>
-      <c r="G23" s="3">
-        <v>1.000020076692967</v>
+      <c r="G23">
+        <v>6.2475036853878181E-2</v>
       </c>
       <c r="H23">
         <v>414</v>
@@ -1481,36 +1705,44 @@
         <v>6.8239999999999998</v>
       </c>
       <c r="J23">
-        <v>3.3860000000000001</v>
+        <v>4.1310000000000002</v>
       </c>
       <c r="K23">
         <v>407.17599999999999</v>
       </c>
       <c r="L23">
-        <v>410.61399999999998</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+        <v>409.86900000000003</v>
+      </c>
+      <c r="N23">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="P23">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16">
       <c r="A24" s="1">
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>33</v>
-      </c>
-      <c r="C24" s="3">
+        <v>36</v>
+      </c>
+      <c r="C24">
         <v>53282</v>
       </c>
-      <c r="D24" s="3">
+      <c r="D24">
         <v>-1</v>
       </c>
-      <c r="E24" s="3">
-        <v>50280.927081875678</v>
-      </c>
-      <c r="F24" s="3">
+      <c r="E24">
+        <v>50010.739068330768</v>
+      </c>
+      <c r="F24">
         <v>1.000018768064262</v>
       </c>
-      <c r="G24" s="3">
-        <v>5.6324329381861077E-2</v>
+      <c r="G24">
+        <v>6.139523538285397E-2</v>
       </c>
       <c r="H24">
         <v>348</v>
@@ -1519,36 +1751,44 @@
         <v>7.524</v>
       </c>
       <c r="J24">
-        <v>7.7720000000000002</v>
+        <v>5.1269999999999998</v>
       </c>
       <c r="K24">
         <v>340.476</v>
       </c>
       <c r="L24">
-        <v>340.22800000000001</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+        <v>342.87299999999999</v>
+      </c>
+      <c r="N24">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="P24">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16">
       <c r="A25" s="1">
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>34</v>
-      </c>
-      <c r="C25" s="3">
+        <v>37</v>
+      </c>
+      <c r="C25">
         <v>36138</v>
       </c>
-      <c r="D25" s="3">
+      <c r="D25">
         <v>35037.496987199193</v>
       </c>
-      <c r="E25" s="3">
-        <v>34929.075115142718</v>
-      </c>
-      <c r="F25" s="3">
+      <c r="E25">
+        <v>35185.827877583331</v>
+      </c>
+      <c r="F25">
         <v>3.0452792429044431E-2</v>
       </c>
-      <c r="G25" s="3">
-        <v>3.3453010262252343E-2</v>
+      <c r="G25">
+        <v>2.634822409698015E-2</v>
       </c>
       <c r="H25">
         <v>62</v>
@@ -1557,36 +1797,44 @@
         <v>10.006</v>
       </c>
       <c r="J25">
-        <v>6.1539999999999999</v>
+        <v>7.7549999999999999</v>
       </c>
       <c r="K25">
         <v>51.994</v>
       </c>
       <c r="L25">
-        <v>55.845999999999997</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+        <v>54.244999999999997</v>
+      </c>
+      <c r="N25">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="P25">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16">
       <c r="A26" s="1">
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>35</v>
-      </c>
-      <c r="C26" s="3">
+        <v>38</v>
+      </c>
+      <c r="C26">
         <v>17776</v>
       </c>
-      <c r="D26" s="3">
+      <c r="D26">
         <v>17273.47893590176</v>
       </c>
-      <c r="E26" s="3">
-        <v>17171.04621726472</v>
-      </c>
-      <c r="F26" s="3">
+      <c r="E26">
+        <v>17155.803586674469</v>
+      </c>
+      <c r="F26">
         <v>2.826963681920815E-2</v>
       </c>
-      <c r="G26" s="3">
-        <v>3.4032053484207687E-2</v>
+      <c r="G26">
+        <v>3.4889537203281473E-2</v>
       </c>
       <c r="H26">
         <v>299</v>
@@ -1595,36 +1843,44 @@
         <v>6.9690000000000003</v>
       </c>
       <c r="J26">
-        <v>3.7869999999999999</v>
+        <v>4.0359999999999996</v>
       </c>
       <c r="K26">
         <v>292.03100000000001</v>
       </c>
       <c r="L26">
-        <v>295.21300000000002</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+        <v>294.964</v>
+      </c>
+      <c r="N26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P26">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16">
       <c r="A27" s="1">
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>36</v>
-      </c>
-      <c r="C27" s="3">
+        <v>39</v>
+      </c>
+      <c r="C27">
         <v>2814</v>
       </c>
-      <c r="D27" s="3">
+      <c r="D27">
         <v>2790.087478868204</v>
       </c>
-      <c r="E27" s="3">
-        <v>2790.5945147205521</v>
-      </c>
-      <c r="F27" s="3">
+      <c r="E27">
+        <v>2773.6274453350779</v>
+      </c>
+      <c r="F27">
         <v>8.4976976303468323E-3</v>
       </c>
-      <c r="G27" s="3">
-        <v>8.3175143139475431E-3</v>
+      <c r="G27">
+        <v>1.4347034351429141E-2</v>
       </c>
       <c r="H27">
         <v>952</v>
@@ -1633,36 +1889,44 @@
         <v>0.44900000000000001</v>
       </c>
       <c r="J27">
-        <v>0.27700000000000002</v>
+        <v>0.34899999999999998</v>
       </c>
       <c r="K27">
         <v>951.55100000000004</v>
       </c>
       <c r="L27">
-        <v>951.72299999999996</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+        <v>951.65099999999995</v>
+      </c>
+      <c r="N27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P27">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16">
       <c r="A28" s="1">
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>37</v>
-      </c>
-      <c r="C28" s="3">
+        <v>40</v>
+      </c>
+      <c r="C28">
         <v>12270</v>
       </c>
-      <c r="D28" s="3">
+      <c r="D28">
         <v>11928.364529941289</v>
       </c>
-      <c r="E28" s="3">
-        <v>11786.82321937704</v>
-      </c>
-      <c r="F28" s="3">
+      <c r="E28">
+        <v>11820.204796235579</v>
+      </c>
+      <c r="F28">
         <v>2.784315159402681E-2</v>
       </c>
-      <c r="G28" s="3">
-        <v>3.9378710727217749E-2</v>
+      <c r="G28">
+        <v>3.6658125816171373E-2</v>
       </c>
       <c r="H28">
         <v>24</v>
@@ -1671,36 +1935,44 @@
         <v>7.194</v>
       </c>
       <c r="J28">
-        <v>4.0519999999999996</v>
+        <v>5.117</v>
       </c>
       <c r="K28">
         <v>16.806000000000001</v>
       </c>
       <c r="L28">
-        <v>19.948</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+        <v>18.882999999999999</v>
+      </c>
+      <c r="N28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P28">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16">
       <c r="A29" s="1">
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>38</v>
-      </c>
-      <c r="C29" s="3">
+        <v>41</v>
+      </c>
+      <c r="C29">
         <v>44419</v>
       </c>
-      <c r="D29" s="3">
+      <c r="D29">
         <v>42623.196511682647</v>
       </c>
-      <c r="E29" s="3">
-        <v>41845.295795560822</v>
-      </c>
-      <c r="F29" s="3">
+      <c r="E29">
+        <v>42486.792561264338</v>
+      </c>
+      <c r="F29">
         <v>4.0428723931591283E-2</v>
       </c>
-      <c r="G29" s="3">
-        <v>5.7941516117858978E-2</v>
+      <c r="G29">
+        <v>4.3499570875878843E-2</v>
       </c>
       <c r="H29">
         <v>6</v>
@@ -1709,36 +1981,44 @@
         <v>7.98</v>
       </c>
       <c r="J29">
-        <v>5.98</v>
+        <v>6.5490000000000004</v>
       </c>
       <c r="K29">
         <v>-1.98</v>
       </c>
       <c r="L29">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+        <v>-0.54900000000000004</v>
+      </c>
+      <c r="N29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P29">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16">
       <c r="A30" s="1">
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>39</v>
-      </c>
-      <c r="C30" s="3">
+        <v>42</v>
+      </c>
+      <c r="C30">
         <v>24121</v>
       </c>
-      <c r="D30" s="3">
+      <c r="D30">
         <v>23356.573902873119</v>
       </c>
-      <c r="E30" s="3">
-        <v>23120.830659237999</v>
-      </c>
-      <c r="F30" s="3">
+      <c r="E30">
+        <v>23167.327646174181</v>
+      </c>
+      <c r="F30">
         <v>3.1691310357235658E-2</v>
       </c>
-      <c r="G30" s="3">
-        <v>4.1464671479706651E-2</v>
+      <c r="G30">
+        <v>3.9537015622313307E-2</v>
       </c>
       <c r="H30">
         <v>356</v>
@@ -1747,36 +2027,44 @@
         <v>9.6140000000000008</v>
       </c>
       <c r="J30">
-        <v>5.4349999999999996</v>
+        <v>6.0830000000000002</v>
       </c>
       <c r="K30">
         <v>346.38600000000002</v>
       </c>
       <c r="L30">
-        <v>350.565</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+        <v>349.91699999999997</v>
+      </c>
+      <c r="N30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P30">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16">
       <c r="A31" s="1">
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>40</v>
-      </c>
-      <c r="C31" s="3">
+        <v>43</v>
+      </c>
+      <c r="C31">
         <v>25782</v>
       </c>
-      <c r="D31" s="3">
+      <c r="D31">
         <v>25052.954362658329</v>
       </c>
-      <c r="E31" s="3">
-        <v>25002.542736253301</v>
-      </c>
-      <c r="F31" s="3">
+      <c r="E31">
+        <v>24984.53448500661</v>
+      </c>
+      <c r="F31">
         <v>2.827731119935099E-2</v>
       </c>
-      <c r="G31" s="3">
-        <v>3.023261437230234E-2</v>
+      <c r="G31">
+        <v>3.0931095919377601E-2</v>
       </c>
       <c r="H31">
         <v>38</v>
@@ -1785,36 +2073,44 @@
         <v>6.0170000000000003</v>
       </c>
       <c r="J31">
-        <v>3.3</v>
+        <v>3.903</v>
       </c>
       <c r="K31">
         <v>31.983000000000001</v>
       </c>
       <c r="L31">
-        <v>34.700000000000003</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+        <v>34.097000000000001</v>
+      </c>
+      <c r="N31">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P31">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16">
       <c r="A32" s="1">
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>41</v>
-      </c>
-      <c r="C32" s="3">
+        <v>44</v>
+      </c>
+      <c r="C32">
         <v>20170</v>
       </c>
-      <c r="D32" s="3">
+      <c r="D32">
         <v>19594.135864279691</v>
       </c>
-      <c r="E32" s="3">
-        <v>19575.359344118879</v>
-      </c>
-      <c r="F32" s="3">
+      <c r="E32">
+        <v>19491.076334233891</v>
+      </c>
+      <c r="F32">
         <v>2.8550527303932011E-2</v>
       </c>
-      <c r="G32" s="3">
-        <v>2.94814405493861E-2</v>
+      <c r="G32">
+        <v>3.3660072670605327E-2</v>
       </c>
       <c r="H32">
         <v>291</v>
@@ -1823,36 +2119,44 @@
         <v>7.4359999999999999</v>
       </c>
       <c r="J32">
-        <v>4.3120000000000003</v>
+        <v>4.6879999999999997</v>
       </c>
       <c r="K32">
         <v>283.56400000000002</v>
       </c>
       <c r="L32">
-        <v>286.68799999999999</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+        <v>286.31200000000001</v>
+      </c>
+      <c r="N32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P32">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16">
       <c r="A33" s="1">
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>42</v>
-      </c>
-      <c r="C33" s="3">
+        <v>45</v>
+      </c>
+      <c r="C33">
         <v>9590</v>
       </c>
-      <c r="D33" s="3">
+      <c r="D33">
         <v>9300.3449429410921</v>
       </c>
-      <c r="E33" s="3">
-        <v>9252.6983185445933</v>
-      </c>
-      <c r="F33" s="3">
+      <c r="E33">
+        <v>9281.3917667090391</v>
+      </c>
+      <c r="F33">
         <v>3.0203864135444E-2</v>
       </c>
-      <c r="G33" s="3">
-        <v>3.5172229557393811E-2</v>
+      <c r="G33">
+        <v>3.2180212021998007E-2</v>
       </c>
       <c r="H33">
         <v>31</v>
@@ -1861,36 +2165,44 @@
         <v>4.6630000000000003</v>
       </c>
       <c r="J33">
-        <v>3.2250000000000001</v>
+        <v>4.665</v>
       </c>
       <c r="K33">
         <v>26.337</v>
       </c>
       <c r="L33">
-        <v>27.774999999999999</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+        <v>26.335000000000001</v>
+      </c>
+      <c r="N33">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16">
       <c r="A34" s="1">
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>43</v>
-      </c>
-      <c r="C34" s="3">
+        <v>46</v>
+      </c>
+      <c r="C34">
         <v>22497</v>
       </c>
-      <c r="D34" s="3">
+      <c r="D34">
         <v>21555.06297733443</v>
       </c>
-      <c r="E34" s="3">
-        <v>21622.068570730749</v>
-      </c>
-      <c r="F34" s="3">
+      <c r="E34">
+        <v>21619.363067866649</v>
+      </c>
+      <c r="F34">
         <v>4.1869450267394158E-2</v>
       </c>
-      <c r="G34" s="3">
-        <v>3.8891026771091727E-2</v>
+      <c r="G34">
+        <v>3.9011287377576913E-2</v>
       </c>
       <c r="H34">
         <v>205</v>
@@ -1899,36 +2211,44 @@
         <v>0.25700000000000001</v>
       </c>
       <c r="J34">
-        <v>3.6880000000000002</v>
+        <v>5.7329999999999997</v>
       </c>
       <c r="K34">
         <v>204.74299999999999</v>
       </c>
       <c r="L34">
-        <v>201.31200000000001</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+        <v>199.267</v>
+      </c>
+      <c r="N34">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="P34">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16">
       <c r="A35" s="1">
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>44</v>
-      </c>
-      <c r="C35" s="3">
+        <v>47</v>
+      </c>
+      <c r="C35">
         <v>18244</v>
       </c>
-      <c r="D35" s="3">
+      <c r="D35">
         <v>17896.42429779932</v>
       </c>
-      <c r="E35" s="3">
-        <v>17783.616024048461</v>
-      </c>
-      <c r="F35" s="3">
+      <c r="E35">
+        <v>17789.169927255389</v>
+      </c>
+      <c r="F35">
         <v>1.9051507465505581E-2</v>
       </c>
-      <c r="G35" s="3">
-        <v>2.5234815607955461E-2</v>
+      <c r="G35">
+        <v>2.4930392060108251E-2</v>
       </c>
       <c r="H35">
         <v>383</v>
@@ -1937,35 +2257,43 @@
         <v>8.3859999999999992</v>
       </c>
       <c r="J35">
-        <v>4.7</v>
+        <v>5.7670000000000003</v>
       </c>
       <c r="K35">
         <v>374.61399999999998</v>
       </c>
       <c r="L35">
-        <v>378.3</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+        <v>377.233</v>
+      </c>
+      <c r="N35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P35">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16">
       <c r="A36" s="1">
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>45</v>
-      </c>
-      <c r="C36" s="3">
+        <v>48</v>
+      </c>
+      <c r="C36">
         <v>32857</v>
       </c>
-      <c r="D36" s="3">
+      <c r="D36">
         <v>32285.1909889913</v>
       </c>
-      <c r="E36" s="3">
+      <c r="E36">
         <v>32285.1909889913</v>
       </c>
-      <c r="F36" s="3">
+      <c r="F36">
         <v>1.740295860878046E-2</v>
       </c>
-      <c r="G36" s="3">
+      <c r="G36">
         <v>1.740295860878046E-2</v>
       </c>
       <c r="H36">
@@ -1975,36 +2303,44 @@
         <v>0.182</v>
       </c>
       <c r="J36">
-        <v>2.36</v>
+        <v>3.194</v>
       </c>
       <c r="K36">
         <v>250.81800000000001</v>
       </c>
       <c r="L36">
-        <v>248.64</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+        <v>247.80600000000001</v>
+      </c>
+      <c r="N36">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="P36">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16">
       <c r="A37" s="1">
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>46</v>
-      </c>
-      <c r="C37" s="3">
+        <v>49</v>
+      </c>
+      <c r="C37">
         <v>4675</v>
       </c>
-      <c r="D37" s="3">
+      <c r="D37">
         <v>4675.5318367192576</v>
       </c>
-      <c r="E37" s="3">
-        <v>4638.9042299613993</v>
-      </c>
-      <c r="F37" s="3">
+      <c r="E37">
+        <v>4622.5783398752419</v>
+      </c>
+      <c r="F37">
         <v>-1.137618650818452E-4</v>
       </c>
-      <c r="G37" s="3">
-        <v>7.7210203291124442E-3</v>
+      <c r="G37">
+        <v>1.1213189331499059E-2</v>
       </c>
       <c r="H37">
         <v>532</v>
@@ -2013,36 +2349,44 @@
         <v>0.94899999999999995</v>
       </c>
       <c r="J37">
-        <v>0.55400000000000005</v>
+        <v>0.59699999999999998</v>
       </c>
       <c r="K37">
         <v>531.05100000000004</v>
       </c>
       <c r="L37">
-        <v>531.44600000000003</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+        <v>531.40300000000002</v>
+      </c>
+      <c r="N37">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P37">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16">
       <c r="A38" s="1">
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>47</v>
-      </c>
-      <c r="C38" s="3">
+        <v>50</v>
+      </c>
+      <c r="C38">
         <v>17886</v>
       </c>
-      <c r="D38" s="3">
+      <c r="D38">
         <v>17357.798173988849</v>
       </c>
-      <c r="E38" s="3">
-        <v>17378.233440365599</v>
-      </c>
-      <c r="F38" s="3">
+      <c r="E38">
+        <v>17377.899969231319</v>
+      </c>
+      <c r="F38">
         <v>2.9531579224597499E-2</v>
       </c>
-      <c r="G38" s="3">
-        <v>2.8389050633702621E-2</v>
+      <c r="G38">
+        <v>2.8407694888107151E-2</v>
       </c>
       <c r="H38">
         <v>429</v>
@@ -2051,36 +2395,44 @@
         <v>0.189</v>
       </c>
       <c r="J38">
-        <v>2.31</v>
+        <v>3.1669999999999998</v>
       </c>
       <c r="K38">
         <v>428.81099999999998</v>
       </c>
       <c r="L38">
-        <v>426.69</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+        <v>425.83300000000003</v>
+      </c>
+      <c r="N38">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="P38">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16">
       <c r="A39" s="1">
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>48</v>
-      </c>
-      <c r="C39" s="3">
+        <v>51</v>
+      </c>
+      <c r="C39">
         <v>21736</v>
       </c>
-      <c r="D39" s="3">
+      <c r="D39">
         <v>20979.37752062282</v>
       </c>
-      <c r="E39" s="3">
-        <v>20870.9147831808</v>
-      </c>
-      <c r="F39" s="3">
+      <c r="E39">
+        <v>20847.394935928201</v>
+      </c>
+      <c r="F39">
         <v>3.4809646640466672E-2</v>
       </c>
-      <c r="G39" s="3">
-        <v>3.9799651123444947E-2</v>
+      <c r="G39">
+        <v>4.0881719914970659E-2</v>
       </c>
       <c r="H39">
         <v>836</v>
@@ -2089,36 +2441,44 @@
         <v>9.7319999999999993</v>
       </c>
       <c r="J39">
-        <v>5.7759999999999998</v>
+        <v>7.7729999999999997</v>
       </c>
       <c r="K39">
         <v>826.26800000000003</v>
       </c>
       <c r="L39">
-        <v>830.22400000000005</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+        <v>828.22699999999998</v>
+      </c>
+      <c r="N39">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P39">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16">
       <c r="A40" s="1">
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>49</v>
-      </c>
-      <c r="C40" s="3">
+        <v>52</v>
+      </c>
+      <c r="C40">
         <v>27464</v>
       </c>
-      <c r="D40" s="3">
+      <c r="D40">
         <v>26864.400845225249</v>
       </c>
-      <c r="E40" s="3">
-        <v>26882.810299396249</v>
-      </c>
-      <c r="F40" s="3">
+      <c r="E40">
+        <v>26733.69940354738</v>
+      </c>
+      <c r="F40">
         <v>2.1832185944317909E-2</v>
       </c>
-      <c r="G40" s="3">
-        <v>2.1161873747587639E-2</v>
+      <c r="G40">
+        <v>2.659119561799533E-2</v>
       </c>
       <c r="H40">
         <v>71</v>
@@ -2127,36 +2487,44 @@
         <v>6.032</v>
       </c>
       <c r="J40">
-        <v>3.7789999999999999</v>
+        <v>4.9930000000000003</v>
       </c>
       <c r="K40">
         <v>64.968000000000004</v>
       </c>
       <c r="L40">
-        <v>67.221000000000004</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+        <v>66.007000000000005</v>
+      </c>
+      <c r="N40">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P40">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16">
       <c r="A41" s="1">
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>50</v>
-      </c>
-      <c r="C41" s="3">
+        <v>53</v>
+      </c>
+      <c r="C41">
         <v>26086</v>
       </c>
-      <c r="D41" s="3">
+      <c r="D41">
         <v>25093.101813511959</v>
       </c>
-      <c r="E41" s="3">
-        <v>24666.179582761179</v>
-      </c>
-      <c r="F41" s="3">
+      <c r="E41">
+        <v>24676.687902788632</v>
+      </c>
+      <c r="F41">
         <v>3.8062492773443389E-2</v>
       </c>
-      <c r="G41" s="3">
-        <v>5.4428445037139513E-2</v>
+      <c r="G41">
+        <v>5.4025611332184642E-2</v>
       </c>
       <c r="H41">
         <v>758</v>
@@ -2165,24 +2533,42 @@
         <v>13.202</v>
       </c>
       <c r="J41">
-        <v>6.8739999999999997</v>
+        <v>6.7759999999999998</v>
       </c>
       <c r="K41">
         <v>744.798</v>
       </c>
       <c r="L41">
-        <v>751.12599999999998</v>
+        <v>751.22400000000005</v>
+      </c>
+      <c r="N41">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P41">
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="F1:G1048576">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
+  <conditionalFormatting sqref="F1:F1048576">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="greaterThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K1:L1048576">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
-      <formula>0</formula>
+  <conditionalFormatting sqref="G1:G1048576">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThan">
+      <formula>0.05</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D1:D1048576">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>-1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E1:E1048576">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>-1</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>